<commit_message>
fix: manual en formato MD agregado y bloques corregidos
fix: manual en formato MD agregado y bloques corregidos
</commit_message>
<xml_diff>
--- a/Practica1/info.xlsx
+++ b/Practica1/info.xlsx
@@ -5,27 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp_gm\Escritorio\PRIMER SEMESTRE 2022\IA\IA\Practica1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp_gm\Escritorio\PRIMER SEMESTRE 2022\IA\IA\Laboratorio_IA\Practica1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEE300B-A00B-41A3-9A2D-ABA7F8D430D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E782BC-1CCB-47F2-9831-7016B6E02D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19305" yWindow="1215" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DPI</t>
   </si>
@@ -34,6 +44,27 @@
   </si>
   <si>
     <t>2564971330101</t>
+  </si>
+  <si>
+    <t>1922100250101</t>
+  </si>
+  <si>
+    <t>20/05/1987</t>
+  </si>
+  <si>
+    <t>201314632</t>
+  </si>
+  <si>
+    <t>24/07/1992</t>
+  </si>
+  <si>
+    <t>15/06/1994</t>
+  </si>
+  <si>
+    <t>02/04/1994</t>
+  </si>
+  <si>
+    <t>2215833350108</t>
   </si>
 </sst>
 </file>
@@ -353,19 +384,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -373,15 +405,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="str">
+        <f>TEXT(B2,"dd/mm/yyyy")</f>
+        <v>24/07/1992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C5" si="0">TEXT(B3,"dd/mm/yyyy")</f>
+        <v>15/06/1994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>20/05/1987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>34426</v>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>02/04/1994</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: final practica 1
fix: final practica 1
</commit_message>
<xml_diff>
--- a/Practica1/info.xlsx
+++ b/Practica1/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp_gm\Escritorio\PRIMER SEMESTRE 2022\IA\IA\Laboratorio_IA\Practica1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E782BC-1CCB-47F2-9831-7016B6E02D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10981127-CD3D-43D5-A273-02AF14811B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="1215" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -61,10 +61,10 @@
     <t>15/06/1994</t>
   </si>
   <si>
-    <t>02/04/1994</t>
-  </si>
-  <si>
     <t>2215833350108</t>
+  </si>
+  <si>
+    <t>04/02/1994</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,14 +407,14 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="str">
         <f>TEXT(B2,"dd/mm/yyyy")</f>
-        <v>24/07/1992</v>
+        <v>04/02/1994</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -425,7 +425,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C5" si="0">TEXT(B3,"dd/mm/yyyy")</f>
+        <f t="shared" ref="C3:C4" si="0">TEXT(B3,"dd/mm/yyyy")</f>
         <v>15/06/1994</v>
       </c>
     </row>
@@ -443,14 +443,14 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>02/04/1994</v>
+        <f>TEXT(B5,"dd/mm/yyyy")</f>
+        <v>24/07/1992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>